<commit_message>
typos in the testcase file fixed
</commit_message>
<xml_diff>
--- a/testcases/IrishNetwork.xlsx
+++ b/testcases/IrishNetwork.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="441" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="441" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="busbar" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="bus" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="demand" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="branch" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="transformer" sheetId="4" state="visible" r:id="rId5"/>
@@ -569,8 +569,8 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="R3:R50 A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -693,7 +693,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="R3:R50 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -744,7 +744,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="1" sqref="R3:R50 D20"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1210,7 +1210,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="R3:R50 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1298,7 +1298,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="R3:R50 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1407,7 +1407,7 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="R3:R50 D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1484,7 +1484,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R3:R50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1521,7 +1521,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="R3:R50 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1668,7 +1668,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="R3:R50 D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1711,10 +1711,10 @@
   </sheetPr>
   <dimension ref="A1:X74"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="R3" activeCellId="0" sqref="R3:R50"/>
+      <selection pane="bottomLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6631,7 +6631,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="R3:R50 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>